<commit_message>
interpolation and annuity calculation with some plots
</commit_message>
<xml_diff>
--- a/LCC/rals_livslangd_python/data/raw/mistra_results_new_structure.xlsx
+++ b/LCC/rals_livslangd_python/data/raw/mistra_results_new_structure.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\rurut\LCC\rals_livslangd_python\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F942EC9A-1C55-4D08-95ED-326CCD76E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADD0636-8ABB-435A-8F82-B25DB496016C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="330" firstSheet="2" activeTab="4" xr2:uid="{3A71664D-9E65-4FDA-91B2-AC2A81079053}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="330" activeTab="2" xr2:uid="{3A71664D-9E65-4FDA-91B2-AC2A81079053}"/>
+    <workbookView xWindow="-28920" yWindow="-10395" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="4" xr2:uid="{263CC2E4-021E-41ED-A6D5-DF2279780A9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Wear-raw" sheetId="1" r:id="rId1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="65">
   <si>
     <t>month 1</t>
   </si>
@@ -214,9 +215,6 @@
     <t>Initially 3 mm</t>
   </si>
   <si>
-    <t>Rail profile</t>
-  </si>
-  <si>
     <t>Gauge</t>
   </si>
   <si>
@@ -233,6 +231,12 @@
   </si>
   <si>
     <t>RCF-residual</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
 </sst>
 </file>
@@ -523,7 +527,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
@@ -541,33 +545,39 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
@@ -8886,6 +8896,7 @@
     <sheetView topLeftCell="E27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB50" sqref="Q47:AB50"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11384,6 +11395,7 @@
     <sheetView topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="Q38" sqref="Q38:AB39"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -13034,9 +13046,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C240127D-17EB-4812-A2BA-3FDC0D42802F}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L15" sqref="K14:L15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" activeCellId="3" sqref="B21:M24 B26:M27 B30:M33 B35:M36"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14430,9 +14443,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CE4E5A-ADD0-4101-BB70-0C5E1C06C9B2}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="A2:M36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15825,689 +15839,735 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29073B79-1DA3-4A22-9289-3455834981DE}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="I1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="M1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="N1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="O1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="P1" s="28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="19">
+      <c r="B2">
+        <v>32.5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="7">
         <v>1440</v>
       </c>
-      <c r="D2" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="E2" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="F2" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="G2" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="H2" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="I2" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="J2" s="20">
-        <v>0.53</v>
-      </c>
-      <c r="K2" s="20">
+      <c r="E2" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="F2" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="G2" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="H2" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="I2" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="J2" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="K2" s="19">
+        <v>0.53</v>
+      </c>
+      <c r="L2" s="19">
         <v>0.73</v>
       </c>
-      <c r="L2" s="20">
+      <c r="M2" s="19">
         <v>0.88</v>
       </c>
-      <c r="M2" s="20">
+      <c r="N2" s="19">
         <v>0.9</v>
       </c>
-      <c r="N2" s="20">
+      <c r="O2" s="19">
         <v>0.94</v>
       </c>
-      <c r="O2" s="21">
+      <c r="P2" s="20">
         <v>1.01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="22">
+      <c r="B3">
+        <v>32.5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="8">
         <v>1445</v>
       </c>
-      <c r="D3" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="E3" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="F3" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="G3" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="H3" s="25">
+      <c r="E3" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="I3" s="23">
         <v>0.54</v>
       </c>
-      <c r="I3" s="25">
+      <c r="J3" s="23">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J3" s="17">
+      <c r="K3" s="17">
         <v>0.56999999999999995</v>
       </c>
-      <c r="K3" s="17">
+      <c r="L3" s="17">
         <v>0.78</v>
       </c>
-      <c r="L3" s="17">
+      <c r="M3" s="17">
         <v>0.88</v>
       </c>
-      <c r="M3" s="17">
+      <c r="N3" s="17">
         <v>0.94</v>
       </c>
-      <c r="N3" s="17">
+      <c r="O3" s="17">
         <v>1</v>
       </c>
-      <c r="O3" s="18">
+      <c r="P3" s="18">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="B4">
+        <v>32.5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="7">
         <v>1450</v>
       </c>
-      <c r="D4" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="F4" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="I4" s="24">
-        <v>0.53</v>
-      </c>
-      <c r="J4" s="20">
+      <c r="E4" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="H4" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="I4" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="J4" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="K4" s="19">
         <v>0.81</v>
       </c>
-      <c r="K4" s="20">
+      <c r="L4" s="19">
         <v>0.9</v>
       </c>
-      <c r="L4" s="20">
+      <c r="M4" s="19">
         <v>0.94</v>
       </c>
-      <c r="M4" s="20">
+      <c r="N4" s="19">
         <v>0.96</v>
       </c>
-      <c r="N4" s="20">
+      <c r="O4" s="19">
         <v>1.06</v>
       </c>
-      <c r="O4" s="21">
+      <c r="P4" s="20">
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="22">
+      <c r="B5">
+        <v>32.5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="8">
         <v>1455</v>
       </c>
-      <c r="D5" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="E5" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="F5" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="G5" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="H5" s="25">
-        <v>0.53</v>
-      </c>
-      <c r="I5" s="25">
+      <c r="E5" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="I5" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="J5" s="23">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J5" s="17">
+      <c r="K5" s="17">
         <v>0.8</v>
       </c>
-      <c r="K5" s="17">
+      <c r="L5" s="17">
         <v>0.91</v>
       </c>
-      <c r="L5" s="17">
+      <c r="M5" s="17">
         <v>1.04</v>
       </c>
-      <c r="M5" s="17">
+      <c r="N5" s="17">
         <v>1.1100000000000001</v>
       </c>
-      <c r="N5" s="17">
+      <c r="O5" s="17">
         <v>1.21</v>
       </c>
-      <c r="O5" s="18">
+      <c r="P5" s="18">
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="34">
+      <c r="B6">
+        <v>32.5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="32">
         <v>1450</v>
       </c>
-      <c r="D6" s="35">
-        <v>0.53</v>
-      </c>
-      <c r="E6" s="35">
-        <v>0.53</v>
-      </c>
-      <c r="F6" s="35">
-        <v>0.53</v>
-      </c>
-      <c r="G6" s="35">
-        <v>0.53</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0.53</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0.53</v>
-      </c>
-      <c r="J6" s="36">
+      <c r="E6" s="33">
+        <v>0.53</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0.53</v>
+      </c>
+      <c r="G6" s="33">
+        <v>0.53</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0.53</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0.53</v>
+      </c>
+      <c r="J6" s="33">
+        <v>0.53</v>
+      </c>
+      <c r="K6" s="34">
         <v>0.82</v>
       </c>
-      <c r="K6" s="36">
+      <c r="L6" s="34">
         <v>0.92</v>
       </c>
-      <c r="L6" s="36">
+      <c r="M6" s="34">
         <v>0.97</v>
       </c>
-      <c r="M6" s="36">
+      <c r="N6" s="34">
         <v>0.98</v>
       </c>
-      <c r="N6" s="36">
+      <c r="O6" s="34">
         <v>1.1100000000000001</v>
       </c>
-      <c r="O6" s="37">
+      <c r="P6" s="35">
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="40">
+      <c r="B7">
+        <v>32.5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="38">
         <v>1455</v>
       </c>
-      <c r="D7" s="41">
-        <v>0.53</v>
-      </c>
-      <c r="E7" s="41">
-        <v>0.53</v>
-      </c>
-      <c r="F7" s="41">
-        <v>0.53</v>
-      </c>
-      <c r="G7" s="41">
-        <v>0.53</v>
-      </c>
-      <c r="H7" s="41">
-        <v>0.53</v>
-      </c>
-      <c r="I7" s="41">
-        <v>0.53</v>
-      </c>
-      <c r="J7" s="42">
+      <c r="E7" s="39">
+        <v>0.53</v>
+      </c>
+      <c r="F7" s="39">
+        <v>0.53</v>
+      </c>
+      <c r="G7" s="39">
+        <v>0.53</v>
+      </c>
+      <c r="H7" s="39">
+        <v>0.53</v>
+      </c>
+      <c r="I7" s="39">
+        <v>0.53</v>
+      </c>
+      <c r="J7" s="39">
+        <v>0.53</v>
+      </c>
+      <c r="K7" s="40">
         <v>0.85</v>
       </c>
-      <c r="K7" s="42">
+      <c r="L7" s="40">
         <v>0.95</v>
       </c>
-      <c r="L7" s="42">
+      <c r="M7" s="40">
         <v>0.98</v>
       </c>
-      <c r="M7" s="42">
+      <c r="N7" s="40">
         <v>1.01</v>
       </c>
-      <c r="N7" s="42">
+      <c r="O7" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="O7" s="43">
+      <c r="P7" s="41">
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="34">
+      <c r="B8">
+        <v>32.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="32">
         <v>1440</v>
       </c>
-      <c r="D8" s="35">
+      <c r="E8" s="33">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E8" s="35">
+      <c r="F8" s="33">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F8" s="35">
+      <c r="G8" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="G8" s="35">
+      <c r="H8" s="33">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="H8" s="35">
+      <c r="I8" s="33">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="I8" s="35">
+      <c r="J8" s="33">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="J8" s="36">
+      <c r="K8" s="34">
         <v>0.20599999999999999</v>
       </c>
-      <c r="K8" s="36">
+      <c r="L8" s="34">
         <v>0.30299999999999999</v>
       </c>
-      <c r="L8" s="36">
+      <c r="M8" s="34">
         <v>0.37</v>
       </c>
-      <c r="M8" s="36">
+      <c r="N8" s="34">
         <v>0.42499999999999999</v>
       </c>
-      <c r="N8" s="36">
+      <c r="O8" s="34">
         <v>0.53700000000000003</v>
       </c>
-      <c r="O8" s="37">
+      <c r="P8" s="35">
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="31">
+      <c r="B9">
+        <v>32.5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="29">
         <v>1445</v>
       </c>
-      <c r="D9" s="32">
+      <c r="E9" s="30">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E9" s="32">
+      <c r="F9" s="30">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F9" s="32">
+      <c r="G9" s="30">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="G9" s="32">
+      <c r="H9" s="30">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="H9" s="32">
+      <c r="I9" s="30">
         <v>0.105</v>
       </c>
-      <c r="I9" s="32">
+      <c r="J9" s="30">
         <v>0.112</v>
       </c>
-      <c r="J9" s="38">
+      <c r="K9" s="36">
         <v>0.249</v>
       </c>
-      <c r="K9" s="33">
+      <c r="L9" s="31">
         <v>0.33500000000000002</v>
       </c>
-      <c r="L9" s="33">
+      <c r="M9" s="31">
         <v>0.433</v>
       </c>
-      <c r="M9" s="33">
+      <c r="N9" s="31">
         <v>0.49299999999999999</v>
       </c>
-      <c r="N9" s="33">
+      <c r="O9" s="31">
         <v>0.61099999999999999</v>
       </c>
-      <c r="O9" s="39">
+      <c r="P9" s="37">
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="22">
+      <c r="B10">
+        <v>32.5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="8">
         <v>1450</v>
       </c>
-      <c r="D10" s="25">
+      <c r="E10" s="23">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="E10" s="25">
+      <c r="F10" s="23">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="F10" s="25">
+      <c r="G10" s="23">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="G10" s="25">
+      <c r="H10" s="23">
         <v>7.8E-2</v>
       </c>
-      <c r="H10" s="25">
+      <c r="I10" s="23">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="I10" s="25">
+      <c r="J10" s="23">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="J10" s="14">
+      <c r="K10" s="14">
         <v>0.25800000000000001</v>
       </c>
-      <c r="K10" s="17">
+      <c r="L10" s="17">
         <v>0.34499999999999997</v>
       </c>
-      <c r="L10" s="17">
+      <c r="M10" s="17">
         <v>0.44600000000000001</v>
       </c>
-      <c r="M10" s="17">
+      <c r="N10" s="17">
         <v>0.54100000000000004</v>
       </c>
-      <c r="N10" s="17">
+      <c r="O10" s="17">
         <v>0.625</v>
       </c>
-      <c r="O10" s="26">
+      <c r="P10" s="24">
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="19">
+      <c r="B11">
+        <v>32.5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="7">
         <v>1455</v>
       </c>
-      <c r="D11" s="24">
+      <c r="E11" s="22">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="E11" s="24">
+      <c r="F11" s="22">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F11" s="24">
+      <c r="G11" s="22">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="G11" s="24">
+      <c r="H11" s="22">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="H11" s="24">
+      <c r="I11" s="22">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="I11" s="24">
+      <c r="J11" s="22">
         <v>0.114</v>
       </c>
-      <c r="J11" s="27">
+      <c r="K11" s="25">
         <v>0.26300000000000001</v>
       </c>
-      <c r="K11" s="20">
+      <c r="L11" s="19">
         <v>0.40100000000000002</v>
       </c>
-      <c r="L11" s="20">
+      <c r="M11" s="19">
         <v>0.53700000000000003</v>
       </c>
-      <c r="M11" s="20">
+      <c r="N11" s="19">
         <v>0.61399999999999999</v>
       </c>
-      <c r="N11" s="20">
+      <c r="O11" s="19">
         <v>0.71299999999999997</v>
       </c>
-      <c r="O11" s="21">
+      <c r="P11" s="20">
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="22">
+      <c r="B12">
+        <v>32.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="8">
         <v>1450</v>
       </c>
-      <c r="D12" s="24">
+      <c r="E12" s="22">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E12" s="24">
+      <c r="F12" s="22">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="F12" s="24">
+      <c r="G12" s="22">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="G12" s="24">
+      <c r="H12" s="22">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="H12" s="24">
+      <c r="I12" s="22">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="I12" s="24">
+      <c r="J12" s="22">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="J12" s="20">
+      <c r="K12" s="19">
         <v>0.24099999999999999</v>
       </c>
-      <c r="K12" s="20">
+      <c r="L12" s="19">
         <v>0.33300000000000002</v>
       </c>
-      <c r="L12" s="20">
+      <c r="M12" s="19">
         <v>0.42899999999999999</v>
       </c>
-      <c r="M12" s="20">
+      <c r="N12" s="19">
         <v>0.52700000000000002</v>
       </c>
-      <c r="N12" s="14">
+      <c r="O12" s="14">
         <v>0.65600000000000003</v>
       </c>
-      <c r="O12" s="15">
+      <c r="P12" s="15">
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="19">
+      <c r="B13">
+        <v>32.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="7">
         <v>1455</v>
       </c>
-      <c r="D13" s="25">
+      <c r="E13" s="23">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E13" s="25">
+      <c r="F13" s="23">
         <v>6.2E-2</v>
       </c>
-      <c r="F13" s="25">
+      <c r="G13" s="23">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G13" s="25">
+      <c r="H13" s="23">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="H13" s="25">
+      <c r="I13" s="23">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I13" s="25">
+      <c r="J13" s="23">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="J13" s="17">
+      <c r="K13" s="17">
         <v>0.26800000000000002</v>
       </c>
-      <c r="K13" s="17">
+      <c r="L13" s="17">
         <v>0.33900000000000002</v>
       </c>
-      <c r="L13" s="17">
+      <c r="M13" s="17">
         <v>0.46400000000000002</v>
       </c>
-      <c r="M13" s="17">
+      <c r="N13" s="17">
         <v>0.54300000000000004</v>
       </c>
-      <c r="N13" s="27">
+      <c r="O13" s="25">
         <v>0.66600000000000004</v>
       </c>
-      <c r="O13" s="26">
+      <c r="P13" s="24">
         <v>0.748</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="22">
+      <c r="B14">
+        <v>32.5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="8">
         <v>1440</v>
       </c>
-      <c r="D14" s="20">
-        <v>0</v>
-      </c>
-      <c r="E14" s="20">
-        <v>0</v>
-      </c>
-      <c r="F14" s="20">
-        <v>0</v>
-      </c>
-      <c r="G14" s="20">
-        <v>0</v>
-      </c>
-      <c r="H14" s="20">
-        <v>0</v>
-      </c>
-      <c r="I14" s="20">
-        <v>0</v>
-      </c>
-      <c r="J14" s="20">
-        <v>0</v>
-      </c>
-      <c r="K14" s="20">
-        <v>0</v>
-      </c>
-      <c r="L14" s="20">
-        <v>0</v>
-      </c>
-      <c r="M14" s="20">
-        <v>0</v>
-      </c>
-      <c r="N14" s="20">
-        <v>0</v>
-      </c>
-      <c r="O14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E14" s="19">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0</v>
+      </c>
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="19">
+        <v>0</v>
+      </c>
+      <c r="I14" s="19">
+        <v>0</v>
+      </c>
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0</v>
+      </c>
+      <c r="L14" s="19">
+        <v>0</v>
+      </c>
+      <c r="M14" s="19">
+        <v>0</v>
+      </c>
+      <c r="N14" s="19">
+        <v>0</v>
+      </c>
+      <c r="O14" s="19">
+        <v>0</v>
+      </c>
+      <c r="P14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="19">
+      <c r="B15">
+        <v>32.5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="7">
         <v>1445</v>
       </c>
-      <c r="D15" s="17">
-        <v>0</v>
-      </c>
       <c r="E15" s="17">
         <v>0</v>
       </c>
@@ -16538,70 +16598,76 @@
       <c r="N15" s="17">
         <v>0</v>
       </c>
-      <c r="O15" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O15" s="17">
+        <v>0</v>
+      </c>
+      <c r="P15" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="22">
+      <c r="B16">
+        <v>32.5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="8">
         <v>1450</v>
       </c>
-      <c r="D16" s="20">
-        <v>0</v>
-      </c>
-      <c r="E16" s="20">
-        <v>0</v>
-      </c>
-      <c r="F16" s="20">
-        <v>0</v>
-      </c>
-      <c r="G16" s="20">
-        <v>0</v>
-      </c>
-      <c r="H16" s="20">
-        <v>0</v>
-      </c>
-      <c r="I16" s="20">
-        <v>0</v>
-      </c>
-      <c r="J16" s="20">
-        <v>0</v>
-      </c>
-      <c r="K16" s="20">
-        <v>0</v>
-      </c>
-      <c r="L16" s="20">
+      <c r="E16" s="19">
+        <v>0</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="19">
+        <v>0</v>
+      </c>
+      <c r="I16" s="19">
+        <v>0</v>
+      </c>
+      <c r="J16" s="19">
+        <v>0</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19">
+        <v>0</v>
+      </c>
+      <c r="M16" s="19">
         <v>0.11</v>
       </c>
-      <c r="M16" s="20">
+      <c r="N16" s="19">
         <v>0.27</v>
       </c>
-      <c r="N16" s="20">
+      <c r="O16" s="19">
         <v>0.35</v>
       </c>
-      <c r="O16" s="21">
+      <c r="P16" s="20">
         <v>0.45</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="19">
+      <c r="B17">
+        <v>32.5</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="7">
         <v>1455</v>
       </c>
-      <c r="D17" s="17">
-        <v>0</v>
-      </c>
       <c r="E17" s="17">
         <v>0</v>
       </c>
@@ -16621,34 +16687,37 @@
         <v>0</v>
       </c>
       <c r="K17" s="17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="17">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L17" s="17">
+      <c r="M17" s="17">
         <v>0.24</v>
       </c>
-      <c r="M17" s="17">
+      <c r="N17" s="17">
         <v>0.36</v>
       </c>
-      <c r="N17" s="17">
+      <c r="O17" s="17">
         <v>0.55000000000000004</v>
       </c>
-      <c r="O17" s="18">
+      <c r="P17" s="18">
         <v>0.67</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="22">
+      <c r="B18">
+        <v>32.5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="8">
         <v>1450</v>
       </c>
-      <c r="D18" s="17">
-        <v>0</v>
-      </c>
       <c r="E18" s="17">
         <v>0</v>
       </c>
@@ -16671,345 +16740,1569 @@
         <v>0</v>
       </c>
       <c r="L18" s="17">
+        <v>0</v>
+      </c>
+      <c r="M18" s="17">
         <v>0.01</v>
       </c>
-      <c r="M18" s="17">
+      <c r="N18" s="17">
         <v>0.02</v>
       </c>
-      <c r="N18" s="17">
+      <c r="O18" s="17">
         <v>0.2</v>
       </c>
-      <c r="O18" s="18">
+      <c r="P18" s="18">
         <v>0.27</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="19">
+      <c r="B19">
+        <v>32.5</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="7">
         <v>1455</v>
       </c>
-      <c r="D19" s="20">
-        <v>0</v>
-      </c>
-      <c r="E19" s="20">
-        <v>0</v>
-      </c>
-      <c r="F19" s="20">
-        <v>0</v>
-      </c>
-      <c r="G19" s="20">
-        <v>0</v>
-      </c>
-      <c r="H19" s="20">
-        <v>0</v>
-      </c>
-      <c r="I19" s="20">
-        <v>0</v>
-      </c>
-      <c r="J19" s="20">
-        <v>0</v>
-      </c>
-      <c r="K19" s="20">
+      <c r="E19" s="19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19">
         <v>0.11</v>
       </c>
-      <c r="L19" s="20">
+      <c r="M19" s="19">
         <v>0.35</v>
       </c>
-      <c r="M19" s="20">
+      <c r="N19" s="19">
         <v>0.63</v>
       </c>
-      <c r="N19" s="20">
+      <c r="O19" s="19">
         <v>0.79</v>
       </c>
-      <c r="O19" s="21">
+      <c r="P19" s="20">
         <v>0.99</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="22">
+      <c r="B20">
+        <v>32.5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="8">
         <v>1440</v>
       </c>
-      <c r="D20" s="25">
+      <c r="E20" s="23">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E20" s="25">
+      <c r="F20" s="23">
         <v>2.0400000000000001E-2</v>
       </c>
-      <c r="F20" s="25">
+      <c r="G20" s="23">
         <v>3.3599999999999998E-2</v>
       </c>
-      <c r="G20" s="25">
+      <c r="H20" s="23">
         <v>4.7E-2</v>
       </c>
-      <c r="H20" s="25">
+      <c r="I20" s="23">
         <v>5.6500000000000002E-2</v>
       </c>
-      <c r="I20" s="25">
+      <c r="J20" s="23">
         <v>6.6100000000000006E-2</v>
       </c>
-      <c r="J20" s="17">
+      <c r="K20" s="17">
         <v>0.1212</v>
       </c>
-      <c r="K20" s="14">
+      <c r="L20" s="14">
         <v>0.18720000000000001</v>
       </c>
-      <c r="L20" s="14">
+      <c r="M20" s="14">
         <v>0.24299999999999999</v>
       </c>
-      <c r="M20" s="14">
+      <c r="N20" s="14">
         <v>0.30020000000000002</v>
       </c>
-      <c r="N20" s="14">
+      <c r="O20" s="14">
         <v>0.34410000000000002</v>
       </c>
-      <c r="O20" s="15">
+      <c r="P20" s="15">
         <v>0.42</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="19">
+      <c r="B21">
+        <v>32.5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="7">
         <v>1445</v>
       </c>
-      <c r="D21" s="24">
+      <c r="E21" s="22">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="E21" s="24">
+      <c r="F21" s="22">
         <v>2.3199999999999998E-2</v>
       </c>
-      <c r="F21" s="24">
+      <c r="G21" s="22">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="G21" s="24">
+      <c r="H21" s="22">
         <v>4.7199999999999999E-2</v>
       </c>
-      <c r="H21" s="24">
+      <c r="I21" s="22">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="I21" s="24">
+      <c r="J21" s="22">
         <v>8.0199999999999994E-2</v>
       </c>
-      <c r="J21" s="20">
+      <c r="K21" s="19">
         <v>0.1318</v>
       </c>
-      <c r="K21" s="27">
+      <c r="L21" s="25">
         <v>0.19819999999999999</v>
       </c>
-      <c r="L21" s="27">
+      <c r="M21" s="25">
         <v>0.28920000000000001</v>
       </c>
-      <c r="M21" s="27">
+      <c r="N21" s="25">
         <v>0.3826</v>
       </c>
-      <c r="N21" s="27">
+      <c r="O21" s="25">
         <v>0.45350000000000001</v>
       </c>
-      <c r="O21" s="26">
+      <c r="P21" s="24">
         <v>0.52339999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="22">
+      <c r="B22">
+        <v>32.5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="8">
         <v>1450</v>
       </c>
-      <c r="D22" s="25">
+      <c r="E22" s="23">
         <v>2.7199999999999998E-2</v>
       </c>
-      <c r="E22" s="25">
+      <c r="F22" s="23">
         <v>4.7399999999999998E-2</v>
       </c>
-      <c r="F22" s="25">
+      <c r="G22" s="23">
         <v>6.5600000000000006E-2</v>
       </c>
-      <c r="G22" s="25">
+      <c r="H22" s="23">
         <v>8.2299999999999998E-2</v>
       </c>
-      <c r="H22" s="25">
+      <c r="I22" s="23">
         <v>9.7600000000000006E-2</v>
       </c>
-      <c r="I22" s="25">
+      <c r="J22" s="23">
         <v>0.1135</v>
       </c>
-      <c r="J22" s="17">
+      <c r="K22" s="17">
         <v>0.3105</v>
       </c>
-      <c r="K22" s="27">
+      <c r="L22" s="25">
         <v>0.43690000000000001</v>
       </c>
-      <c r="L22" s="27">
+      <c r="M22" s="25">
         <v>0.58540000000000003</v>
       </c>
-      <c r="M22" s="27">
+      <c r="N22" s="25">
         <v>0.70579999999999998</v>
       </c>
-      <c r="N22" s="27">
+      <c r="O22" s="25">
         <v>0.81259999999999999</v>
       </c>
-      <c r="O22" s="26">
+      <c r="P22" s="24">
         <v>0.9234</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23">
+        <v>32.5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1455</v>
+      </c>
+      <c r="E23" s="22">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="F23" s="22">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="G23" s="22">
+        <v>9.8199999999999996E-2</v>
+      </c>
+      <c r="H23" s="22">
+        <v>0.1203</v>
+      </c>
+      <c r="I23" s="22">
+        <v>0.15260000000000001</v>
+      </c>
+      <c r="J23" s="22">
+        <v>0.2064</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0.39639999999999997</v>
+      </c>
+      <c r="L23" s="19">
+        <v>0.58169999999999999</v>
+      </c>
+      <c r="M23" s="19">
+        <v>0.79</v>
+      </c>
+      <c r="N23" s="19">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="O23" s="19">
+        <v>1.1195999999999999</v>
+      </c>
+      <c r="P23" s="20">
+        <v>1.244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>32.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1450</v>
+      </c>
+      <c r="E24" s="22">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F24" s="22">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="G24" s="22">
+        <v>5.1499999999999997E-2</v>
+      </c>
+      <c r="H24" s="22">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="I24" s="22">
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="J24" s="22">
+        <v>9.5899999999999999E-2</v>
+      </c>
+      <c r="K24" s="19">
+        <v>0.21790000000000001</v>
+      </c>
+      <c r="L24" s="19">
+        <v>0.379</v>
+      </c>
+      <c r="M24" s="19">
+        <v>0.53139999999999998</v>
+      </c>
+      <c r="N24" s="19">
+        <v>0.64280000000000004</v>
+      </c>
+      <c r="O24" s="19">
+        <v>0.75480000000000003</v>
+      </c>
+      <c r="P24" s="20">
+        <v>0.83389999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25">
+        <v>32.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1455</v>
+      </c>
+      <c r="E25" s="23">
+        <v>2.98E-2</v>
+      </c>
+      <c r="F25" s="23">
+        <v>6.93E-2</v>
+      </c>
+      <c r="G25" s="23">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="H25" s="23">
+        <v>0.121</v>
+      </c>
+      <c r="I25" s="23">
+        <v>0.1434</v>
+      </c>
+      <c r="J25" s="23">
+        <v>0.1739</v>
+      </c>
+      <c r="K25" s="17">
+        <v>0.37809999999999999</v>
+      </c>
+      <c r="L25" s="17">
+        <v>0.67789999999999995</v>
+      </c>
+      <c r="M25" s="17">
+        <v>0.85870000000000002</v>
+      </c>
+      <c r="N25" s="17">
+        <v>1.0952999999999999</v>
+      </c>
+      <c r="O25" s="17">
+        <v>1.2991999999999999</v>
+      </c>
+      <c r="P25" s="18">
+        <v>1.5158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1440</v>
+      </c>
+      <c r="E26" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="F26" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="G26" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="H26" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="I26" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="J26" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="K26" s="19">
+        <v>0.74</v>
+      </c>
+      <c r="L26" s="19">
+        <v>0.85</v>
+      </c>
+      <c r="M26" s="19">
+        <v>0.88</v>
+      </c>
+      <c r="N26" s="19">
+        <v>0.92</v>
+      </c>
+      <c r="O26" s="19">
+        <v>0.95</v>
+      </c>
+      <c r="P26" s="20">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1445</v>
+      </c>
+      <c r="E27" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="G27" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="H27" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="I27" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="J27" s="23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K27" s="17">
+        <v>0.74</v>
+      </c>
+      <c r="L27" s="17">
+        <v>0.88</v>
+      </c>
+      <c r="M27" s="17">
+        <v>0.89</v>
+      </c>
+      <c r="N27" s="17">
+        <v>0.98</v>
+      </c>
+      <c r="O27" s="17">
+        <v>1.06</v>
+      </c>
+      <c r="P27" s="18">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1450</v>
+      </c>
+      <c r="E28" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="F28" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="G28" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="H28" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="I28" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="J28" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="K28" s="19">
+        <v>0.89</v>
+      </c>
+      <c r="L28" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="M28" s="19">
+        <v>0.99</v>
+      </c>
+      <c r="N28" s="19">
+        <v>1.03</v>
+      </c>
+      <c r="O28" s="19">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P28" s="20">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>30</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1455</v>
+      </c>
+      <c r="E29" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="G29" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="H29" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="I29" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="J29" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="K29" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="L29" s="17">
+        <v>0.98</v>
+      </c>
+      <c r="M29" s="17">
+        <v>0.99</v>
+      </c>
+      <c r="N29" s="17">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="O29" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="P29" s="18">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="32">
+        <v>1450</v>
+      </c>
+      <c r="E30" s="44">
+        <v>0.53</v>
+      </c>
+      <c r="F30" s="44">
+        <v>0.53</v>
+      </c>
+      <c r="G30" s="44">
+        <v>0.53</v>
+      </c>
+      <c r="H30" s="44">
+        <v>0.53</v>
+      </c>
+      <c r="I30" s="44">
+        <v>0.53</v>
+      </c>
+      <c r="J30" s="44">
+        <v>0.53</v>
+      </c>
+      <c r="K30" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="L30" s="44">
+        <v>0.88</v>
+      </c>
+      <c r="M30" s="44">
+        <v>0.89</v>
+      </c>
+      <c r="N30" s="44">
+        <v>0.96</v>
+      </c>
+      <c r="O30" s="44">
+        <v>1.06</v>
+      </c>
+      <c r="P30" s="45">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="38">
+        <v>1455</v>
+      </c>
+      <c r="E31" s="42">
+        <v>0.53</v>
+      </c>
+      <c r="F31" s="42">
+        <v>0.53</v>
+      </c>
+      <c r="G31" s="42">
+        <v>0.53</v>
+      </c>
+      <c r="H31" s="42">
+        <v>0.53</v>
+      </c>
+      <c r="I31" s="42">
+        <v>0.53</v>
+      </c>
+      <c r="J31" s="42">
+        <v>0.53</v>
+      </c>
+      <c r="K31" s="42">
+        <v>0.7</v>
+      </c>
+      <c r="L31" s="42">
+        <v>0.86</v>
+      </c>
+      <c r="M31" s="42">
+        <v>0.89</v>
+      </c>
+      <c r="N31" s="42">
+        <v>0.94</v>
+      </c>
+      <c r="O31" s="42">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P31" s="43">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="32">
+        <v>1440</v>
+      </c>
+      <c r="E32" s="46">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F32" s="46">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G32" s="46">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="H32" s="46">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="I32" s="46">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J32" s="46">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="K32" s="44">
+        <v>0.216</v>
+      </c>
+      <c r="L32" s="44">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="M32" s="44">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="N32" s="44">
+        <v>0.48</v>
+      </c>
+      <c r="O32" s="44">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="P32" s="45">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="29">
+        <v>1445</v>
+      </c>
+      <c r="E33" s="46">
+        <v>0.05</v>
+      </c>
+      <c r="F33" s="46">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G33" s="46">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H33" s="46">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="I33" s="46">
+        <v>0.1</v>
+      </c>
+      <c r="J33" s="46">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="K33" s="14">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="L33" s="14">
+        <v>0.33</v>
+      </c>
+      <c r="M33" s="14">
+        <v>0.433</v>
+      </c>
+      <c r="N33" s="42">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="O33" s="42">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="P33" s="43">
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="8">
+        <v>1450</v>
+      </c>
+      <c r="E34" s="46">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F34" s="46">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G34" s="46">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="H34" s="46">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="I34" s="46">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J34" s="46">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="K34" s="47">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="L34" s="14">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="M34" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="N34" s="14">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="O34" s="14">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="P34" s="45">
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1455</v>
+      </c>
+      <c r="E35" s="46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F35" s="46">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="G35" s="46">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H35" s="46">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I35" s="46">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="J35" s="46">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="K35" s="47">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="L35" s="47">
+        <v>0.373</v>
+      </c>
+      <c r="M35" s="47">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="N35" s="47">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="O35" s="47">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="P35" s="43">
+        <v>0.80900000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="8">
+        <v>1450</v>
+      </c>
+      <c r="E36" s="42">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F36" s="42">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G36" s="42">
+        <v>0.08</v>
+      </c>
+      <c r="H36" s="42">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="I36" s="42">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="J36" s="42">
+        <v>0.104</v>
+      </c>
+      <c r="K36" s="14">
+        <v>0.18</v>
+      </c>
+      <c r="L36" s="14">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="M36" s="14">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="N36" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="O36" s="14">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="P36" s="43">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1455</v>
+      </c>
+      <c r="E37" s="44">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F37" s="44">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G37" s="44">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H37" s="44">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I37" s="44">
+        <v>0.08</v>
+      </c>
+      <c r="J37" s="44">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="K37" s="47">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="L37" s="47">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="M37" s="47">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="N37" s="47">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="O37" s="47">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="P37" s="45">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="19">
+      <c r="D38" s="8">
+        <v>1440</v>
+      </c>
+      <c r="E38" s="48">
+        <v>0</v>
+      </c>
+      <c r="F38" s="48">
+        <v>0</v>
+      </c>
+      <c r="G38" s="48">
+        <v>0</v>
+      </c>
+      <c r="H38" s="48">
+        <v>0</v>
+      </c>
+      <c r="I38" s="48">
+        <v>0</v>
+      </c>
+      <c r="J38" s="48">
+        <v>0</v>
+      </c>
+      <c r="K38" s="42">
+        <v>0</v>
+      </c>
+      <c r="L38" s="42">
+        <v>0</v>
+      </c>
+      <c r="M38" s="42">
+        <v>0</v>
+      </c>
+      <c r="N38" s="42">
+        <v>0</v>
+      </c>
+      <c r="O38" s="42">
+        <v>0</v>
+      </c>
+      <c r="P38" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>30</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="7">
+        <v>1445</v>
+      </c>
+      <c r="E39" s="48">
+        <v>0</v>
+      </c>
+      <c r="F39" s="48">
+        <v>0</v>
+      </c>
+      <c r="G39" s="48">
+        <v>0</v>
+      </c>
+      <c r="H39" s="48">
+        <v>0</v>
+      </c>
+      <c r="I39" s="48">
+        <v>0</v>
+      </c>
+      <c r="J39" s="48">
+        <v>0</v>
+      </c>
+      <c r="K39" s="44">
+        <v>0</v>
+      </c>
+      <c r="L39" s="44">
+        <v>0</v>
+      </c>
+      <c r="M39" s="44">
+        <v>0</v>
+      </c>
+      <c r="N39" s="44">
+        <v>0</v>
+      </c>
+      <c r="O39" s="44">
+        <v>0</v>
+      </c>
+      <c r="P39" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>30</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="8">
+        <v>1450</v>
+      </c>
+      <c r="E40" s="48">
+        <v>0</v>
+      </c>
+      <c r="F40" s="48">
+        <v>0</v>
+      </c>
+      <c r="G40" s="48">
+        <v>0</v>
+      </c>
+      <c r="H40" s="48">
+        <v>0</v>
+      </c>
+      <c r="I40" s="48">
+        <v>0</v>
+      </c>
+      <c r="J40" s="48">
+        <v>0</v>
+      </c>
+      <c r="K40" s="42">
+        <v>0</v>
+      </c>
+      <c r="L40" s="42">
+        <v>0</v>
+      </c>
+      <c r="M40" s="42">
+        <v>0.17</v>
+      </c>
+      <c r="N40" s="42">
+        <v>0.21</v>
+      </c>
+      <c r="O40" s="42">
+        <v>0.3</v>
+      </c>
+      <c r="P40" s="43">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="7">
         <v>1455</v>
       </c>
-      <c r="D23" s="24">
-        <v>3.2800000000000003E-2</v>
-      </c>
-      <c r="E23" s="24">
-        <v>6.4600000000000005E-2</v>
-      </c>
-      <c r="F23" s="24">
-        <v>9.8199999999999996E-2</v>
-      </c>
-      <c r="G23" s="24">
-        <v>0.1203</v>
-      </c>
-      <c r="H23" s="24">
+      <c r="E41" s="48">
+        <v>0</v>
+      </c>
+      <c r="F41" s="48">
+        <v>0</v>
+      </c>
+      <c r="G41" s="48">
+        <v>0</v>
+      </c>
+      <c r="H41" s="48">
+        <v>0</v>
+      </c>
+      <c r="I41" s="48">
+        <v>0</v>
+      </c>
+      <c r="J41" s="48">
+        <v>0</v>
+      </c>
+      <c r="K41" s="44">
+        <v>0</v>
+      </c>
+      <c r="L41" s="44">
+        <v>0.11</v>
+      </c>
+      <c r="M41" s="44">
+        <v>0.46</v>
+      </c>
+      <c r="N41" s="44">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O41" s="44">
+        <v>0.77</v>
+      </c>
+      <c r="P41" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="8">
+        <v>1450</v>
+      </c>
+      <c r="E42" s="48">
+        <v>0</v>
+      </c>
+      <c r="F42" s="48">
+        <v>0</v>
+      </c>
+      <c r="G42" s="48">
+        <v>0</v>
+      </c>
+      <c r="H42" s="48">
+        <v>0</v>
+      </c>
+      <c r="I42" s="48">
+        <v>0</v>
+      </c>
+      <c r="J42" s="48">
+        <v>0</v>
+      </c>
+      <c r="K42" s="44">
+        <v>0</v>
+      </c>
+      <c r="L42" s="44">
+        <v>0</v>
+      </c>
+      <c r="M42" s="44">
+        <v>0</v>
+      </c>
+      <c r="N42" s="44">
+        <v>0.03</v>
+      </c>
+      <c r="O42" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="P42" s="45">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>30</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="7">
+        <v>1455</v>
+      </c>
+      <c r="E43" s="48">
+        <v>0</v>
+      </c>
+      <c r="F43" s="48">
+        <v>0</v>
+      </c>
+      <c r="G43" s="48">
+        <v>0</v>
+      </c>
+      <c r="H43" s="48">
+        <v>0</v>
+      </c>
+      <c r="I43" s="48">
+        <v>0</v>
+      </c>
+      <c r="J43" s="48">
+        <v>0</v>
+      </c>
+      <c r="K43" s="42">
+        <v>0</v>
+      </c>
+      <c r="L43" s="42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M43" s="42">
+        <v>0.37</v>
+      </c>
+      <c r="N43" s="42">
+        <v>0.64</v>
+      </c>
+      <c r="O43" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="P43" s="43">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>30</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="8">
+        <v>1440</v>
+      </c>
+      <c r="E44" s="46">
+        <v>1.03E-2</v>
+      </c>
+      <c r="F44" s="46">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="G44" s="46">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="H44" s="46">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="I44" s="46">
+        <v>4.6899999999999997E-2</v>
+      </c>
+      <c r="J44" s="46">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="K44" s="14">
+        <v>0.1221</v>
+      </c>
+      <c r="L44" s="14">
+        <v>0.16639999999999999</v>
+      </c>
+      <c r="M44" s="14">
+        <v>0.2001</v>
+      </c>
+      <c r="N44" s="14">
+        <v>0.25019999999999998</v>
+      </c>
+      <c r="O44" s="14">
+        <v>0.29220000000000002</v>
+      </c>
+      <c r="P44" s="15">
+        <v>0.32050000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1445</v>
+      </c>
+      <c r="E45" s="46">
+        <v>1.24E-2</v>
+      </c>
+      <c r="F45" s="46">
+        <v>2.07E-2</v>
+      </c>
+      <c r="G45" s="46">
+        <v>2.7E-2</v>
+      </c>
+      <c r="H45" s="46">
+        <v>3.73E-2</v>
+      </c>
+      <c r="I45" s="46">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="J45" s="46">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="K45" s="47">
+        <v>0.1273</v>
+      </c>
+      <c r="L45" s="47">
+        <v>0.2344</v>
+      </c>
+      <c r="M45" s="47">
+        <v>0.30690000000000001</v>
+      </c>
+      <c r="N45" s="47">
+        <v>0.37740000000000001</v>
+      </c>
+      <c r="O45" s="47">
+        <v>0.43020000000000003</v>
+      </c>
+      <c r="P45" s="49">
+        <v>0.48130000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="8">
+        <v>1450</v>
+      </c>
+      <c r="E46" s="46">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="F46" s="46">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="G46" s="46">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="H46" s="46">
+        <v>8.4699999999999998E-2</v>
+      </c>
+      <c r="I46" s="46">
+        <v>0.1026</v>
+      </c>
+      <c r="J46" s="46">
+        <v>0.1149</v>
+      </c>
+      <c r="K46" s="44">
+        <v>0.25309999999999999</v>
+      </c>
+      <c r="L46" s="44">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="M46" s="44">
+        <v>0.57210000000000005</v>
+      </c>
+      <c r="N46" s="44">
+        <v>0.69079999999999997</v>
+      </c>
+      <c r="O46" s="44">
+        <v>0.82030000000000003</v>
+      </c>
+      <c r="P46" s="45">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="7">
+        <v>1455</v>
+      </c>
+      <c r="E47" s="46">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="F47" s="46">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G47" s="46">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="H47" s="46">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="I47" s="46">
         <v>0.15260000000000001</v>
       </c>
-      <c r="I23" s="24">
-        <v>0.2064</v>
-      </c>
-      <c r="J23" s="20">
-        <v>0.39639999999999997</v>
-      </c>
-      <c r="K23" s="20">
-        <v>0.58169999999999999</v>
-      </c>
-      <c r="L23" s="20">
-        <v>0.79</v>
-      </c>
-      <c r="M23" s="20">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="N23" s="20">
-        <v>1.1195999999999999</v>
-      </c>
-      <c r="O23" s="21">
-        <v>1.244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+      <c r="J47" s="46">
+        <v>0.1842</v>
+      </c>
+      <c r="K47" s="42">
+        <v>0.46360000000000001</v>
+      </c>
+      <c r="L47" s="42">
+        <v>0.71530000000000005</v>
+      </c>
+      <c r="M47" s="42">
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="N47" s="42">
+        <v>1.0884</v>
+      </c>
+      <c r="O47" s="42">
+        <v>1.3346</v>
+      </c>
+      <c r="P47" s="43">
+        <v>1.5916999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="22">
+      <c r="B48">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="8">
         <v>1450</v>
       </c>
-      <c r="D24" s="24">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E24" s="24">
-        <v>3.3399999999999999E-2</v>
-      </c>
-      <c r="F24" s="24">
-        <v>5.1499999999999997E-2</v>
-      </c>
-      <c r="G24" s="24">
-        <v>6.3600000000000004E-2</v>
-      </c>
-      <c r="H24" s="24">
-        <v>7.7799999999999994E-2</v>
-      </c>
-      <c r="I24" s="24">
-        <v>9.5899999999999999E-2</v>
-      </c>
-      <c r="J24" s="20">
-        <v>0.21790000000000001</v>
-      </c>
-      <c r="K24" s="20">
-        <v>0.379</v>
-      </c>
-      <c r="L24" s="20">
-        <v>0.53139999999999998</v>
-      </c>
-      <c r="M24" s="20">
-        <v>0.64280000000000004</v>
-      </c>
-      <c r="N24" s="20">
-        <v>0.75480000000000003</v>
-      </c>
-      <c r="O24" s="21">
-        <v>0.83389999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="E48" s="46">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F48" s="46">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="G48" s="46">
+        <v>5.28E-2</v>
+      </c>
+      <c r="H48" s="46">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I48" s="46">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="J48" s="46">
+        <v>9.3100000000000002E-2</v>
+      </c>
+      <c r="K48" s="42">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="L48" s="42">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="M48" s="42">
+        <v>0.41849999999999998</v>
+      </c>
+      <c r="N48" s="42">
+        <v>0.48680000000000001</v>
+      </c>
+      <c r="O48" s="42">
+        <v>0.53310000000000002</v>
+      </c>
+      <c r="P48" s="43">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="19">
+      <c r="B49">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="7">
         <v>1455</v>
       </c>
-      <c r="D25" s="25">
-        <v>2.98E-2</v>
-      </c>
-      <c r="E25" s="25">
-        <v>6.93E-2</v>
-      </c>
-      <c r="F25" s="25">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="G25" s="25">
-        <v>0.121</v>
-      </c>
-      <c r="H25" s="25">
-        <v>0.1434</v>
-      </c>
-      <c r="I25" s="25">
-        <v>0.1739</v>
-      </c>
-      <c r="J25" s="17">
-        <v>0.37809999999999999</v>
-      </c>
-      <c r="K25" s="17">
-        <v>0.67789999999999995</v>
-      </c>
-      <c r="L25" s="17">
-        <v>0.85870000000000002</v>
-      </c>
-      <c r="M25" s="17">
-        <v>1.0952999999999999</v>
-      </c>
-      <c r="N25" s="17">
-        <v>1.2991999999999999</v>
-      </c>
-      <c r="O25" s="18">
-        <v>1.5158</v>
+      <c r="E49" s="46">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="F49" s="46">
+        <v>5.5800000000000002E-2</v>
+      </c>
+      <c r="G49" s="46">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="H49" s="46">
+        <v>0.11650000000000001</v>
+      </c>
+      <c r="I49" s="46">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J49" s="46">
+        <v>0.1663</v>
+      </c>
+      <c r="K49" s="44">
+        <v>0.31119999999999998</v>
+      </c>
+      <c r="L49" s="44">
+        <v>0.57040000000000002</v>
+      </c>
+      <c r="M49" s="44">
+        <v>0.79090000000000005</v>
+      </c>
+      <c r="N49" s="44">
+        <v>1.0187999999999999</v>
+      </c>
+      <c r="O49" s="44">
+        <v>1.2443</v>
+      </c>
+      <c r="P49" s="45">
+        <v>1.4316</v>
       </c>
     </row>
   </sheetData>
@@ -17024,6 +18317,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>